<commit_message>
modification on weighted avg method
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pengcheng/Desktop/FYP/Improvement-to-Naive-Bayes-Classifier/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DEF8BCD-7763-B14B-91ED-97A2F27799BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C99645D-99FF-D640-A38A-0E4A4F4864B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{C62220F6-D869-944C-BA84-A28CF5D1FDE6}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14540" xr2:uid="{C62220F6-D869-944C-BA84-A28CF5D1FDE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Dataset</t>
   </si>
@@ -57,6 +57,15 @@
   </si>
   <si>
     <t>adult.csv</t>
+  </si>
+  <si>
+    <t>(searched by simulated annealing algorithm)</t>
+  </si>
+  <si>
+    <t>heart.csv</t>
+  </si>
+  <si>
+    <t>Clustered comonotonicity</t>
   </si>
 </sst>
 </file>
@@ -408,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D172D3F1-1305-1D49-8DB9-5F4844304FAE}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -421,9 +430,10 @@
     <col min="3" max="3" width="28.33203125" customWidth="1"/>
     <col min="4" max="4" width="44" customWidth="1"/>
     <col min="5" max="5" width="40.5" customWidth="1"/>
+    <col min="6" max="6" width="38.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -437,10 +447,13 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -454,7 +467,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -468,9 +481,32 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
+      </c>
+      <c r="B4">
+        <v>0.78437754271765603</v>
+      </c>
+      <c r="C4">
+        <v>0.75866558177379895</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>0.86885245901639296</v>
+      </c>
+      <c r="C5">
+        <v>0.52459016393442603</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
backup before big change in clustered comonotonic
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pengcheng/Desktop/FYP/Improvement-to-Naive-Bayes-Classifier/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C99645D-99FF-D640-A38A-0E4A4F4864B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CEF1CA-C051-0649-B55C-EA30613F8216}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14540" xr2:uid="{C62220F6-D869-944C-BA84-A28CF5D1FDE6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{C62220F6-D869-944C-BA84-A28CF5D1FDE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Dataset</t>
   </si>
@@ -47,9 +47,6 @@
     <t>glass.csv</t>
   </si>
   <si>
-    <t>Num of categories for continuous variables</t>
-  </si>
-  <si>
     <t>Weighted avg of Naïve Bayes &amp; Comonotonicity</t>
   </si>
   <si>
@@ -57,9 +54,6 @@
   </si>
   <si>
     <t>adult.csv</t>
-  </si>
-  <si>
-    <t>(searched by simulated annealing algorithm)</t>
   </si>
   <si>
     <t>heart.csv</t>
@@ -420,7 +414,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -428,9 +422,9 @@
     <col min="1" max="1" width="14.6640625" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
     <col min="3" max="3" width="28.33203125" customWidth="1"/>
-    <col min="4" max="4" width="44" customWidth="1"/>
-    <col min="5" max="5" width="40.5" customWidth="1"/>
-    <col min="6" max="6" width="38.5" customWidth="1"/>
+    <col min="4" max="4" width="40.5" customWidth="1"/>
+    <col min="5" max="5" width="38.5" customWidth="1"/>
+    <col min="6" max="6" width="38.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -443,14 +437,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -463,50 +454,44 @@
       <c r="C2">
         <v>0.62790697674418605</v>
       </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>0.93826815642458095</v>
       </c>
       <c r="C3">
         <v>0.92011173184357498</v>
-      </c>
-      <c r="D3">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>0.78437754271765603</v>
+        <v>0.81741253051261098</v>
       </c>
       <c r="C4">
-        <v>0.75866558177379895</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
+        <v>0.45598047192839702</v>
+      </c>
+      <c r="E4">
+        <v>0.812042310821806</v>
+      </c>
+      <c r="F4">
+        <v>0.83970707892595597</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>0.86885245901639296</v>
       </c>
       <c r="C5">
         <v>0.52459016393442603</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>